<commit_message>
Add Occhino lab + fixes
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaalexander/github/rlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82851A7-7769-044A-B6B9-7A33E3D9A089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDBC063-24BB-C94A-B918-C7107D6B4895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7620" yWindow="680" windowWidth="20820" windowHeight="15900" xr2:uid="{59A264FB-7A95-E842-AEEA-C35557593B53}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="189">
   <si>
     <t>Baorian</t>
   </si>
@@ -526,9 +526,6 @@
     <t>Obert</t>
   </si>
   <si>
-    <t>Tiago</t>
-  </si>
-  <si>
     <t>Cardoso Aguiar</t>
   </si>
   <si>
@@ -593,6 +590,18 @@
   </si>
   <si>
     <t>Cho</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>WCP 4.134</t>
+  </si>
+  <si>
+    <t>4.110/W8</t>
+  </si>
+  <si>
+    <t>Thiago</t>
   </si>
 </sst>
 </file>
@@ -963,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17483530-688E-B14A-9F3B-5498A1C19FFD}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,16 +1000,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" t="s">
         <v>168</v>
-      </c>
-      <c r="B2" t="s">
-        <v>169</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D2" s="4" t="str">
-        <f t="shared" ref="D2:D36" si="0">CONCATENATE(A2, " ", B2, "   ", C2)</f>
+        <f t="shared" ref="D2:D37" si="0">CONCATENATE(A2, " ", B2, "   ", C2)</f>
         <v>Akshay Aitha   4.706</v>
       </c>
     </row>
@@ -1111,10 +1120,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" t="s">
         <v>174</v>
-      </c>
-      <c r="B10" t="s">
-        <v>175</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -1126,17 +1135,17 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" t="s">
         <v>163</v>
-      </c>
-      <c r="B11" t="s">
-        <v>164</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Tiago Cardoso Aguiar   W9</v>
+        <v>Thiago Cardoso Aguiar   W9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1156,10 +1165,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" t="s">
         <v>184</v>
-      </c>
-      <c r="B13" t="s">
-        <v>185</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>84</v>
@@ -1216,757 +1225,772 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>185</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>102</v>
+        <v>186</v>
       </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Ashwini Deo   4.426</v>
+        <v>Meg Davis   WCP 4.134</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>102</v>
       </c>
       <c r="D18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Sampada Deshpande   W5</v>
+        <v>Ashwini Deo   4.426</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Pattie Epps   4.736</v>
+        <v>Sampada Deshpande   W5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="D20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Teagan Esther   E7</v>
+        <v>Pattie Epps   4.736</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>James Fazio   4.622</v>
+        <v>Teagan Esther   E7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="D22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Gabriel Gallinate   E8</v>
+        <v>James Fazio   4.622</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="D23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Barrett Hamp   W12</v>
+        <v>Gabriel Gallinate   E8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Leticia Hanada   W10</v>
+        <v>Barrett Hamp   W12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="D25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Ethan Hartzell   E3</v>
+        <v>Leticia Hanada   W10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="D26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Juan Pablo Jáuregui Magrina   (NA)</v>
+        <v>Ethan Hartzell   E3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="D27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Taylor Joyce   W11</v>
+        <v>Juan Pablo Jáuregui Magrina   (NA)</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Anushri Kartik-Narajan   4.110</v>
+        <v>Taylor Joyce   W11</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="D29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Danny Law   4.432</v>
+        <v>Anushri Kartik-Narajan   4.110</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Rebecca Le Borgne   4.624</v>
+        <v>Danny Law   4.432</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="D31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Sooji Lee   E6</v>
+        <v>Rebecca Le Borgne   4.624</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>139</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="D32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Jessy Li   4.728</v>
+        <v>Sooji Lee   E6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Fernando Llanos   4.730</v>
+        <v>Jessy Li   4.728</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="D34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Kyle Mahowald   4.430</v>
+        <v>Fernando Llanos   4.730</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="D35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Rebecca Marcus   4.304C</v>
+        <v>Kyle Mahowald   4.430</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="D36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Richard Meier   4.732</v>
+        <v>Rebecca Marcus   4.304C</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="D37" s="4" t="str">
-        <f t="shared" ref="D37:D66" si="1">CONCATENATE(A37, " ", B37, "   ", C37)</f>
-        <v>Don Miller   4.618</v>
+        <f t="shared" si="0"/>
+        <v>Richard Meier   4.732</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>165</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D38" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Kanishka Misra   4.428</v>
+        <f t="shared" ref="D38:D67" si="1">CONCATENATE(A38, " ", B38, "   ", C38)</f>
+        <v>Don Miller   4.618</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="D39" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Kaiji Mo   W1</v>
+        <v>Kanishka Misra   4.428</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>138</v>
+        <v>5</v>
       </c>
       <c r="D40" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Scott Myers   4.726</v>
+        <v>Kaiji Mo   W1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>42</v>
+        <v>138</v>
       </c>
       <c r="D41" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Lillian Nguyen   FD</v>
+        <v>Scott Myers   4.726</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D42" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Baorian Nuchged   4.110</v>
+        <v>Lillian Nguyen   FD</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="D43" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Karol Obert   4.734</v>
+        <v>Baorian Nuchged   4.110/W8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="D44" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Corrine Occhino   4.704</v>
+        <v>Karol Obert   4.734</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="D45" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Lee Orfila   W8</v>
+        <v>Corrine Occhino   4.704</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D46" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Youn-Gyu Park   W7</v>
+        <v>Lee Orfila   W8</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
         <v>22</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="D47" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>SeYeon Park   E10</v>
+        <v>Youn-Gyu Park   W7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>22</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>167</v>
+        <v>76</v>
       </c>
       <c r="D48" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Justin Power   4.740</v>
+        <v>SeYeon Park   E10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
       <c r="D49" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>David Quinto-Pozos   4.714</v>
+        <v>Justin Power   4.740</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="D50" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Ben Rapstine   4.304D</v>
+        <v>David Quinto-Pozos   4.714</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>180</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>47</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="D51" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Hongjin Ren   (NA)</v>
+        <v>Ben Rapstine   4.304D</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D52" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Oscar Rojas   E8</v>
+        <v>Hongjin Ren   (NA)</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>182</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D53" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Catalina Santamaria Soto   E12</v>
+        <v>Oscar Rojas   E8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="D54" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Jefferson Saransig   W13</v>
+        <v>Catalina Santamaria Soto   E12</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>173</v>
+        <v>38</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D55" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Ari Schifman   E2</v>
+        <v>Jefferson Saransig   W13</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D56" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Will Sheffield   W4</v>
+        <v>Ari Schifman   E2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="D57" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Rajka Smiljanić   4.724</v>
+        <v>Will Sheffield   W4</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>133</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="D58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Madeline Smith   (NA)</v>
+        <v>Rajka Smiljanić   4.724</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="D59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Steve Wechsler   4.702</v>
+        <v>Madeline Smith   (NA)</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B60" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Debbie White   4.620</v>
+        <v>Steve Wechsler   4.702</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Elijah Wilder   E11</v>
+        <v>Debbie White   4.620</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="D62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Tony Woodbury   4.738</v>
+        <v>Elijah Wilder   E11</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>96</v>
+        <v>153</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="D63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Michael Wynne   4.626</v>
+        <v>Tony Woodbury   4.738</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="D64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Qing Yao   W6</v>
+        <v>Michael Wynne   4.626</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="D65" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Hongli Zhan   (NA)</v>
+        <v>Qing Yao   W6</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Hongli Zhan   (NA)</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>49</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>50</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="4" t="str">
+      <c r="D67" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Asher Zheng   W3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D66">
-    <sortCondition ref="B3:B66"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D67">
+    <sortCondition ref="B3:B67"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>